<commit_message>
Fixat mest PCB saker
</commit_message>
<xml_diff>
--- a/Övrigt/Nätlista TXV-11 rev-01.xlsx
+++ b/Övrigt/Nätlista TXV-11 rev-01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="20160" windowHeight="14130"/>
@@ -384,8 +384,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,7 +505,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -540,7 +539,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -716,14 +714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -741,7 +739,7 @@
     <col min="28" max="29" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -800,7 +798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -817,7 +815,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -834,7 +832,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -851,7 +849,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -868,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -888,7 +886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -902,7 +900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -913,7 +911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -924,7 +922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -941,7 +939,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -961,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -972,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -983,7 +981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -1000,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -1017,7 +1015,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1028,7 +1026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1039,7 +1037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1053,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1067,7 +1065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -1084,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1110,7 +1108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1136,7 +1134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -1162,7 +1160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24">
       <c r="C30" t="s">
         <v>33</v>
       </c>
@@ -1170,7 +1168,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24">
       <c r="C31" t="s">
         <v>34</v>
       </c>
@@ -1178,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1195,7 +1193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1212,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29">
       <c r="C34" t="s">
         <v>37</v>
       </c>
@@ -1220,7 +1218,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29">
       <c r="C35" t="s">
         <v>38</v>
       </c>
@@ -1228,7 +1226,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29">
       <c r="C36" t="s">
         <v>39</v>
       </c>
@@ -1236,7 +1234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29">
       <c r="C37" t="s">
         <v>40</v>
       </c>
@@ -1244,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29">
       <c r="C38" t="s">
         <v>41</v>
       </c>
@@ -1252,7 +1250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29">
       <c r="C39" t="s">
         <v>42</v>
       </c>
@@ -1260,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29">
       <c r="C40" t="s">
         <v>43</v>
       </c>
@@ -1268,7 +1266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29">
       <c r="C41" t="s">
         <v>44</v>
       </c>
@@ -1276,7 +1274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29">
       <c r="C42" t="s">
         <v>45</v>
       </c>
@@ -1284,7 +1282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1295,7 +1293,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1306,7 +1304,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -1320,7 +1318,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -1331,7 +1329,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -1342,7 +1340,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -1383,7 +1381,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1433,24 +1431,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
massa saker, Kortet klart för test
</commit_message>
<xml_diff>
--- a/Övrigt/Nätlista TXV-11 rev-01.xlsx
+++ b/Övrigt/Nätlista TXV-11 rev-01.xlsx
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>